<commit_message>
Changed Excel to Scriptable Object
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/ExcelData.xlsx
+++ b/Assets/Editor/Data/ExcelData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="17980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-456" windowWidth="23256" windowHeight="14616"/>
   </bookViews>
   <sheets>
     <sheet name="질문지" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>캐릭터 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,24 +116,36 @@
   </si>
   <si>
     <t xml:space="preserve">말 돌리지마! 모르면 그냥 확실하게 말하라고! </t>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -149,7 +161,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -158,7 +170,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -172,6 +184,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,7 +222,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -215,11 +235,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="열어 본 하이퍼링크" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,23 +543,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.296875" customWidth="1"/>
+    <col min="5" max="5" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.69921875" customWidth="1"/>
+    <col min="8" max="8" width="24.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,38 +585,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="4">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>2</v>
       </c>
@@ -619,7 +656,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -632,18 +669,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="66.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -657,7 +694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>1</v>
       </c>
@@ -668,7 +705,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>2</v>
       </c>
@@ -679,13 +716,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
@@ -710,7 +747,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add bum and face look loading algorithm
hi hi
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/ExcelData.xlsx
+++ b/Assets/Editor/Data/ExcelData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
   <si>
     <t>대사</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>주말이라서 그런지 영화관 안은 커플이나 가족 단위 손님으로 북적인다.</t>
-  </si>
-  <si>
-    <t>#FADE IN</t>
   </si>
   <si>
     <t>#북적거리는 소음</t>
@@ -264,9 +261,6 @@
     <t>히로인_놀람</t>
   </si>
   <si>
-    <t>히로인_뾰루퉁</t>
-  </si>
-  <si>
     <t>저번에도 그렇게 말해놓고선, 여자친구는 내 몫까지 다 샀었지.</t>
   </si>
   <si>
@@ -286,6 +280,9 @@
   </si>
   <si>
     <t>실패시 S#</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
@@ -699,7 +696,7 @@
   <dimension ref="A1:AD998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection sqref="A1:AD998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -716,7 +713,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="16">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -777,13 +774,13 @@
         <v>17</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -798,18 +795,18 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
+      <c r="G2" s="1" t="s">
+        <v>87</v>
       </c>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -842,15 +839,15 @@
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -884,17 +881,17 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -928,15 +925,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -971,12 +968,12 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1007,33 +1004,33 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1062,22 +1059,22 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1106,14 +1103,16 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1146,14 +1145,16 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1186,17 +1187,17 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1227,71 +1228,73 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1">
         <v>17</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="W12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="X12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="Y12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Y12" s="3" t="s">
+      <c r="Z12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -1306,62 +1309,62 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="R13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -1376,62 +1379,62 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="T14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Y14" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="Z14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -1447,59 +1450,59 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="K15" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="L15" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="M15" s="1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="N15" s="1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="O15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="P15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="1">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="R15" s="1">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="S15" s="1">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="T15" s="1">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="U15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="V15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="W15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="X15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="Y15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="Z15" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -1515,59 +1518,59 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="K16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="M16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="N16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="O16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="P16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="R16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="S16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="T16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="U16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="V16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="W16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="X16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="Y16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="Z16" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>

</xml_diff>

<commit_message>
Now we can control sound
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/ExcelData.xlsx
+++ b/Assets/Editor/Data/ExcelData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
   <si>
     <t>대사</t>
   </si>
@@ -81,16 +81,10 @@
     <t>주말이라서 그런지 영화관 안은 커플이나 가족 단위 손님으로 북적인다.</t>
   </si>
   <si>
-    <t>#북적거리는 소음</t>
-  </si>
-  <si>
     <t>"사람 되게 많다."</t>
   </si>
   <si>
     <t>"번호표 미리 뽑아놓을까?"</t>
-  </si>
-  <si>
-    <t>#BGM</t>
   </si>
   <si>
     <t>"당연한 거 아니야? 딱히 고마운 건 아니고…!"</t>
@@ -130,9 +124,6 @@
   </si>
   <si>
     <t>"음… 요즘 어떤게 재미있지? 오빠가 골라줘."</t>
-  </si>
-  <si>
-    <t>#BGM OFF</t>
   </si>
   <si>
     <t>QR</t>
@@ -275,6 +266,12 @@
   <si>
     <t>image_test</t>
   </si>
+  <si>
+    <t>BGM_Light</t>
+  </si>
+  <si>
+    <t>BGM_Fright</t>
+  </si>
 </sst>
 </file>
 
@@ -360,8 +357,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -415,17 +418,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,7 +733,7 @@
   <dimension ref="A1:AD998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -745,7 +750,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="16">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -806,13 +811,13 @@
         <v>17</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -827,17 +832,17 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -871,15 +876,15 @@
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -913,17 +918,15 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -957,15 +960,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1000,12 +1003,12 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1036,33 +1039,33 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1091,22 +1094,22 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1135,15 +1138,15 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1177,15 +1180,15 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1219,17 +1222,15 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1260,73 +1261,75 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1">
         <v>17</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="O12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="U12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="W12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="Y12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="Z12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -1341,62 +1344,62 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="P13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z13" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -1411,62 +1414,62 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="N14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="P14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="S14" s="2" t="s">
+      <c r="Z14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -1482,7 +1485,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1">
@@ -1550,7 +1553,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1">

</xml_diff>

<commit_message>
Character Face Change updated
</commit_message>
<xml_diff>
--- a/Assets/Editor/Data/ExcelData.xlsx
+++ b/Assets/Editor/Data/ExcelData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="질문지" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>대사</t>
   </si>
@@ -81,10 +81,19 @@
     <t>주말이라서 그런지 영화관 안은 커플이나 가족 단위 손님으로 북적인다.</t>
   </si>
   <si>
+    <t>#FADE IN</t>
+  </si>
+  <si>
+    <t>#북적거리는 소음</t>
+  </si>
+  <si>
     <t>"사람 되게 많다."</t>
   </si>
   <si>
     <t>"번호표 미리 뽑아놓을까?"</t>
+  </si>
+  <si>
+    <t>#BGM</t>
   </si>
   <si>
     <t>"당연한 거 아니야? 딱히 고마운 건 아니고…!"</t>
@@ -124,6 +133,9 @@
   </si>
   <si>
     <t>"음… 요즘 어떤게 재미있지? 오빠가 골라줘."</t>
+  </si>
+  <si>
+    <t>#BGM OFF</t>
   </si>
   <si>
     <t>QR</t>
@@ -261,23 +273,26 @@
     <t>실패시 S#</t>
   </si>
   <si>
-    <t>Character</t>
+    <t>Face3</t>
   </si>
   <si>
-    <t>image_test</t>
+    <t>Face1</t>
   </si>
   <si>
-    <t>BGM_Light</t>
+    <t>Face5</t>
   </si>
   <si>
-    <t>BGM_Fright</t>
+    <t>Face4</t>
+  </si>
+  <si>
+    <t>Face6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +349,12 @@
       <charset val="129"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color theme="1"/>
       <name val="굴림"/>
@@ -357,7 +378,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -373,32 +394,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -417,20 +414,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -733,7 +725,7 @@
   <dimension ref="A1:AD998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -746,11 +738,13 @@
     <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="16">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -811,13 +805,13 @@
         <v>17</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
@@ -832,18 +826,18 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="5" t="s">
-        <v>82</v>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>80</v>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
       </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -876,15 +870,15 @@
         <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="5" t="s">
-        <v>80</v>
+      <c r="G3" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -918,15 +912,17 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -960,15 +956,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="5" t="s">
-        <v>80</v>
+      <c r="G5" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1003,12 +999,12 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="5" t="s">
-        <v>80</v>
+      <c r="G6" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1039,33 +1035,33 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
-        <v>81</v>
+      <c r="G7" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1">
         <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1093,23 +1089,23 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="5" t="s">
-        <v>80</v>
+      <c r="G8" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1138,16 +1134,14 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1180,16 +1174,14 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1222,15 +1214,17 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="5" t="s">
-        <v>80</v>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1261,75 +1255,71 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1">
         <v>17</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>43</v>
+      <c r="Q12" s="3" t="s">
+        <v>47</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>44</v>
+      <c r="R12" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -1343,63 +1333,63 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="5" t="s">
-        <v>80</v>
+      <c r="G13" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="N13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="V13" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -1413,63 +1403,63 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="5" t="s">
-        <v>80</v>
+      <c r="G14" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="R14" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="T14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="W14" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
@@ -1485,59 +1475,59 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="K15" s="1">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="L15" s="1">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="M15" s="1">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="N15" s="1">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="O15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="P15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="Q15" s="1">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="R15" s="1">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="S15" s="1">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="T15" s="1">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="U15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="V15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="W15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="X15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="Y15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="Z15" s="1">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -1550,62 +1540,62 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="K16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="L16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="M16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="N16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="O16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="P16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="R16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="S16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="T16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="U16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="V16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="W16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="X16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="Y16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="Z16" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>

</xml_diff>